<commit_message>
WIP CQL, Questionnaire changes
</commit_message>
<xml_diff>
--- a/input/l2/MBODA.xlsx
+++ b/input/l2/MBODA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work/Documents/GitHub/cqf-us/input/l2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonevans/Documents/GitHub/cqf-us/input/l2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262CF0A0-601A-4E41-BD37-6A91A4748C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67276E0D-5C9C-244B-B31A-C6B89B0E79FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1989,7 +1989,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2069,6 +2069,101 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="7" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="10" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2081,9 +2176,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2092,138 +2193,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="7" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="10" borderId="7" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2238,58 +2207,7 @@
     <cellStyle name="Normal 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Normal 3" xfId="7" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -2686,106 +2604,106 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:64" ht="101.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
     </row>
     <row r="4" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
     </row>
     <row r="6" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.15">
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
     </row>
     <row r="10" spans="1:64" ht="31.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="63" t="s">
         <v>216</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -2903,16 +2821,16 @@
       <c r="B12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -2973,16 +2891,16 @@
       <c r="B13" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="65" t="s">
         <v>170</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -3043,16 +2961,16 @@
       <c r="B14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -3113,16 +3031,16 @@
       <c r="B15" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="65" t="s">
         <v>217</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -3628,7 +3546,7 @@
       <c r="A2" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="61" t="s">
         <v>297</v>
       </c>
       <c r="C2" s="28" t="s">
@@ -3657,14 +3575,14 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="71" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="71" t="s">
+    <row r="5" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="60" t="s">
         <v>141</v>
       </c>
-      <c r="C5" s="71" t="s">
+      <c r="C5" s="60" t="s">
         <v>149</v>
       </c>
     </row>
@@ -3761,11 +3679,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="249" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -3799,28 +3717,28 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="57" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="38" t="s">
+      <c r="C6" s="67"/>
+      <c r="D6" s="68" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="38"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="68"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="38"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="68"/>
     </row>
     <row r="9" spans="2:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="38"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="68"/>
     </row>
     <row r="10" spans="2:7" ht="144" x14ac:dyDescent="0.15">
       <c r="B10" s="10" t="s">
@@ -3841,7 +3759,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="67" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="13"/>
@@ -3850,7 +3768,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="16" x14ac:dyDescent="0.15">
-      <c r="B13" s="33"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="15" t="s">
         <v>18</v>
       </c>
@@ -3859,7 +3777,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="32" x14ac:dyDescent="0.15">
-      <c r="B14" s="33"/>
+      <c r="B14" s="67"/>
       <c r="C14" s="15" t="s">
         <v>20</v>
       </c>
@@ -3868,7 +3786,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="48" x14ac:dyDescent="0.15">
-      <c r="B15" s="33"/>
+      <c r="B15" s="67"/>
       <c r="C15" s="17" t="s">
         <v>22</v>
       </c>
@@ -3877,7 +3795,7 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="67" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="13"/>
@@ -3886,7 +3804,7 @@
       </c>
     </row>
     <row r="17" spans="2:4" ht="16" x14ac:dyDescent="0.15">
-      <c r="B17" s="33"/>
+      <c r="B17" s="67"/>
       <c r="C17" s="15" t="s">
         <v>26</v>
       </c>
@@ -3895,7 +3813,7 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="16" x14ac:dyDescent="0.15">
-      <c r="B18" s="33"/>
+      <c r="B18" s="67"/>
       <c r="C18" s="15" t="s">
         <v>28</v>
       </c>
@@ -3904,7 +3822,7 @@
       </c>
     </row>
     <row r="19" spans="2:4" ht="32" x14ac:dyDescent="0.15">
-      <c r="B19" s="33"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="15" t="s">
         <v>30</v>
       </c>
@@ -3913,7 +3831,7 @@
       </c>
     </row>
     <row r="20" spans="2:4" ht="32" x14ac:dyDescent="0.15">
-      <c r="B20" s="33"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="15" t="s">
         <v>32</v>
       </c>
@@ -3922,7 +3840,7 @@
       </c>
     </row>
     <row r="21" spans="2:4" ht="32" x14ac:dyDescent="0.15">
-      <c r="B21" s="33"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="15" t="s">
         <v>34</v>
       </c>
@@ -3931,7 +3849,7 @@
       </c>
     </row>
     <row r="22" spans="2:4" ht="16" x14ac:dyDescent="0.15">
-      <c r="B22" s="33"/>
+      <c r="B22" s="67"/>
       <c r="C22" s="15" t="s">
         <v>36</v>
       </c>
@@ -3940,21 +3858,21 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="135.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="33"/>
-      <c r="C23" s="34" t="s">
+      <c r="B23" s="67"/>
+      <c r="C23" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="70" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="35"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="70"/>
     </row>
     <row r="25" spans="2:4" ht="64" x14ac:dyDescent="0.15">
-      <c r="B25" s="33"/>
+      <c r="B25" s="67"/>
       <c r="C25" s="15" t="s">
         <v>40</v>
       </c>
@@ -3963,7 +3881,7 @@
       </c>
     </row>
     <row r="26" spans="2:4" ht="32" x14ac:dyDescent="0.15">
-      <c r="B26" s="33"/>
+      <c r="B26" s="67"/>
       <c r="C26" s="15" t="s">
         <v>42</v>
       </c>
@@ -3972,7 +3890,7 @@
       </c>
     </row>
     <row r="27" spans="2:4" ht="80" x14ac:dyDescent="0.15">
-      <c r="B27" s="33"/>
+      <c r="B27" s="67"/>
       <c r="C27" s="15" t="s">
         <v>44</v>
       </c>
@@ -3981,7 +3899,7 @@
       </c>
     </row>
     <row r="28" spans="2:4" ht="64" x14ac:dyDescent="0.15">
-      <c r="B28" s="33"/>
+      <c r="B28" s="67"/>
       <c r="C28" s="15" t="s">
         <v>46</v>
       </c>
@@ -3990,16 +3908,16 @@
       </c>
     </row>
     <row r="29" spans="2:4" ht="65.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="33"/>
-      <c r="C29" s="36" t="s">
+      <c r="B29" s="67"/>
+      <c r="C29" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="36"/>
+      <c r="D29" s="71"/>
     </row>
     <row r="30" spans="2:4" ht="61.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="33"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
     </row>
     <row r="31" spans="2:4" ht="64" x14ac:dyDescent="0.15">
       <c r="B31" s="10" t="s">
@@ -4020,7 +3938,7 @@
       </c>
     </row>
     <row r="33" spans="2:4" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="33" t="s">
+      <c r="B33" s="67" t="s">
         <v>53</v>
       </c>
       <c r="C33" s="22" t="s">
@@ -4031,7 +3949,7 @@
       </c>
     </row>
     <row r="34" spans="2:4" ht="48" x14ac:dyDescent="0.15">
-      <c r="B34" s="33"/>
+      <c r="B34" s="67"/>
       <c r="C34" s="15" t="s">
         <v>56</v>
       </c>
@@ -4040,7 +3958,7 @@
       </c>
     </row>
     <row r="35" spans="2:4" ht="48" x14ac:dyDescent="0.15">
-      <c r="B35" s="33"/>
+      <c r="B35" s="67"/>
       <c r="C35" s="15" t="s">
         <v>58</v>
       </c>
@@ -4049,7 +3967,7 @@
       </c>
     </row>
     <row r="36" spans="2:4" ht="32" x14ac:dyDescent="0.15">
-      <c r="B36" s="33"/>
+      <c r="B36" s="67"/>
       <c r="C36" s="9" t="s">
         <v>60</v>
       </c>
@@ -4076,7 +3994,7 @@
       </c>
     </row>
     <row r="39" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B39" s="33" t="s">
+      <c r="B39" s="67" t="s">
         <v>66</v>
       </c>
       <c r="C39" s="13"/>
@@ -4085,7 +4003,7 @@
       </c>
     </row>
     <row r="40" spans="2:4" ht="16" x14ac:dyDescent="0.15">
-      <c r="B40" s="33"/>
+      <c r="B40" s="67"/>
       <c r="C40" s="15" t="s">
         <v>68</v>
       </c>
@@ -4094,7 +4012,7 @@
       </c>
     </row>
     <row r="41" spans="2:4" ht="16" x14ac:dyDescent="0.15">
-      <c r="B41" s="33"/>
+      <c r="B41" s="67"/>
       <c r="C41" s="15" t="s">
         <v>70</v>
       </c>
@@ -4103,7 +4021,7 @@
       </c>
     </row>
     <row r="42" spans="2:4" ht="16" x14ac:dyDescent="0.15">
-      <c r="B42" s="33"/>
+      <c r="B42" s="67"/>
       <c r="C42" s="9" t="s">
         <v>72</v>
       </c>
@@ -4149,17 +4067,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="B12:B15"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="B16:B30"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="C29:D30"/>
     <mergeCell ref="B33:B36"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="B12:B15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D23" r:id="rId1" display="Quantity – a number that is associated with a unit of measure outlined in the standard for Unified Code for Units of Measure (UCUM). Quantities can include any number that is associated with a unit, such as “number of past pregnancies”, where “past pregnancies” is the unit of measure (1)._x000a_– If the data type is a “Quantity” there should be an associated sub-type listed in the “Quantity sub-type” column." xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -4175,2313 +4093,2296 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF09DAA-F93A-7E4A-9C32-0E6EF6031F40}">
-  <dimension ref="B1:BG33"/>
+  <dimension ref="B1:AV33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <pane xSplit="11" ySplit="10" topLeftCell="L11" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="W16" sqref="W16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="6" ySplit="2" topLeftCell="G24" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="32" max="32" width="18" customWidth="1"/>
+    <col min="32" max="32" width="37.33203125" customWidth="1"/>
     <col min="35" max="35" width="63.5" customWidth="1"/>
-    <col min="41" max="41" width="10.83203125" style="73"/>
-    <col min="44" max="44" width="13.5" style="73" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.5" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:48" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="69"/>
-      <c r="AC1" s="41"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="42" t="s">
+    <row r="1" spans="2:48" s="29" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="AF1" s="42" t="s">
+      <c r="AF1" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="AG1" s="42" t="s">
+      <c r="AG1" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="43" t="s">
+      <c r="AH1" s="33" t="s">
         <v>85</v>
       </c>
       <c r="AI1" t="s">
         <v>86</v>
       </c>
-      <c r="AJ1" s="42" t="s">
+      <c r="AJ1" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="AK1" s="42" t="s">
+      <c r="AK1" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="AL1" s="42" t="s">
+      <c r="AL1" s="32" t="s">
         <v>89</v>
       </c>
       <c r="AM1"/>
       <c r="AN1"/>
-      <c r="AO1" s="73"/>
+      <c r="AO1"/>
       <c r="AP1"/>
       <c r="AQ1"/>
-      <c r="AR1" s="73"/>
+      <c r="AR1"/>
       <c r="AS1"/>
     </row>
-    <row r="2" spans="2:48" s="40" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="44" t="s">
+    <row r="2" spans="2:48" s="30" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="44" t="s">
+      <c r="I2" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="44" t="s">
+      <c r="K2" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="L2" s="44" t="s">
+      <c r="L2" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="M2" s="44" t="s">
+      <c r="M2" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="N2" s="44" t="s">
+      <c r="N2" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="O2" s="44" t="s">
+      <c r="O2" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="P2" s="44" t="s">
+      <c r="P2" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="Q2" s="45" t="s">
+      <c r="Q2" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="R2" s="45" t="s">
+      <c r="R2" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="S2" s="45" t="s">
+      <c r="S2" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="T2" s="45" t="s">
+      <c r="T2" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="U2" s="45" t="s">
+      <c r="U2" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="V2" s="45" t="s">
+      <c r="V2" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="W2" s="45" t="s">
+      <c r="W2" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="X2" s="45" t="s">
+      <c r="X2" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="Y2" s="45" t="s">
+      <c r="Y2" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="Z2" s="45" t="s">
+      <c r="Z2" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="AA2" s="45" t="s">
+      <c r="AA2" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="AB2" s="45" t="s">
+      <c r="AB2" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="AC2" s="46" t="s">
+      <c r="AC2" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="AD2" s="45" t="s">
+      <c r="AD2" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="AE2" s="47" t="s">
+      <c r="AE2" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="AF2" s="47" t="s">
+      <c r="AF2" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="AG2" s="47" t="s">
+      <c r="AG2" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="AH2" s="48" t="s">
+      <c r="AH2" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="AI2" s="49" t="s">
+      <c r="AI2" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="AJ2" s="47" t="s">
+      <c r="AJ2" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="AK2" s="47" t="s">
+      <c r="AK2" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="AL2" s="47" t="s">
+      <c r="AL2" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="AM2" s="47" t="s">
+      <c r="AM2" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="AN2" s="47" t="s">
+      <c r="AN2" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="AO2" s="47" t="s">
+      <c r="AO2" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="AP2" s="47" t="s">
+      <c r="AP2" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="AQ2" s="47" t="s">
+      <c r="AQ2" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="AR2" s="47" t="s">
+      <c r="AR2" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="AS2" s="47" t="s">
+      <c r="AS2" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="AT2" s="47" t="s">
+      <c r="AT2" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="AU2" s="47" t="s">
+      <c r="AU2" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="AV2" s="47" t="s">
+      <c r="AV2" s="37" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="2:48" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="50" t="s">
+    <row r="3" spans="2:48" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="42" t="s">
         <v>201</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="42" t="s">
         <v>202</v>
       </c>
-      <c r="F3" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" s="39" t="s">
+      <c r="F3" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J3" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K3" s="53" t="s">
+      <c r="H3" s="30"/>
+      <c r="I3" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K3" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L3" s="40" t="s">
+      <c r="L3" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="M3" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="N3" s="40"/>
-      <c r="P3" s="40" t="s">
+      <c r="N3" s="30"/>
+      <c r="P3" s="30" t="s">
         <v>318</v>
       </c>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="54"/>
-      <c r="W3" s="54"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="54"/>
-      <c r="AB3" s="54"/>
-      <c r="AC3" s="41"/>
-      <c r="AD3" s="54"/>
-      <c r="AF3" s="39" t="s">
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="44"/>
+      <c r="V3" s="44"/>
+      <c r="W3" s="44"/>
+      <c r="X3" s="44"/>
+      <c r="Y3" s="44"/>
+      <c r="Z3" s="44"/>
+      <c r="AA3" s="44"/>
+      <c r="AB3" s="44"/>
+      <c r="AC3" s="31"/>
+      <c r="AD3" s="44"/>
+      <c r="AF3" s="29" t="s">
         <v>317</v>
       </c>
-      <c r="AG3" s="39" t="s">
+      <c r="AG3" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="AI3" s="55"/>
-      <c r="AJ3" s="39" t="s">
+      <c r="AI3" s="45"/>
+      <c r="AJ3" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AO3" s="69" t="s">
+      <c r="AO3" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR3" s="70"/>
-    </row>
-    <row r="4" spans="2:48" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="50" t="s">
+      <c r="AR3" s="59"/>
+    </row>
+    <row r="4" spans="2:48" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="44" t="s">
         <v>299</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="F4" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="39" t="s">
+      <c r="F4" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" s="53" t="s">
+      <c r="H4" s="43"/>
+      <c r="I4" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L4" s="54" t="s">
+      <c r="L4" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M4" s="54" t="s">
+      <c r="M4" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="54"/>
-      <c r="S4" s="54"/>
-      <c r="T4" s="54"/>
-      <c r="U4" s="54"/>
-      <c r="V4" s="54"/>
-      <c r="W4" s="54"/>
-      <c r="X4" s="54"/>
-      <c r="Y4" s="54"/>
-      <c r="Z4" s="54"/>
-      <c r="AA4" s="54"/>
-      <c r="AB4" s="54"/>
-      <c r="AC4" s="41"/>
-      <c r="AD4" s="54"/>
-      <c r="AF4" s="39" t="s">
+      <c r="N4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="44"/>
+      <c r="V4" s="44"/>
+      <c r="W4" s="44"/>
+      <c r="X4" s="44"/>
+      <c r="Y4" s="44"/>
+      <c r="Z4" s="44"/>
+      <c r="AA4" s="44"/>
+      <c r="AB4" s="44"/>
+      <c r="AC4" s="31"/>
+      <c r="AD4" s="44"/>
+      <c r="AF4" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="AG4" s="39" t="s">
+      <c r="AG4" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="AI4" s="55" t="s">
+      <c r="AI4" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="AJ4" s="39" t="s">
+      <c r="AJ4" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL4" s="39" t="s">
+      <c r="AL4" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="AO4" s="69" t="s">
+      <c r="AO4" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR4" s="70"/>
-    </row>
-    <row r="5" spans="2:48" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="50" t="s">
+      <c r="AR4" s="59"/>
+    </row>
+    <row r="5" spans="2:48" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="41" t="s">
         <v>191</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="44" t="s">
         <v>300</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="F5" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="39" t="s">
+      <c r="F5" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="53"/>
-      <c r="I5" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K5" s="53" t="s">
+      <c r="H5" s="43"/>
+      <c r="I5" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L5" s="54" t="s">
+      <c r="L5" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M5" s="54" t="s">
+      <c r="M5" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="O5" s="56"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="54"/>
-      <c r="R5" s="54"/>
-      <c r="S5" s="54"/>
-      <c r="T5" s="54"/>
-      <c r="U5" s="54"/>
-      <c r="V5" s="54"/>
-      <c r="W5" s="54"/>
-      <c r="X5" s="54"/>
-      <c r="Y5" s="54"/>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="54"/>
-      <c r="AB5" s="54"/>
-      <c r="AC5" s="41"/>
-      <c r="AD5" s="54"/>
-      <c r="AF5" s="39" t="s">
+      <c r="O5" s="46"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
+      <c r="S5" s="44"/>
+      <c r="T5" s="44"/>
+      <c r="U5" s="44"/>
+      <c r="V5" s="44"/>
+      <c r="W5" s="44"/>
+      <c r="X5" s="44"/>
+      <c r="Y5" s="44"/>
+      <c r="Z5" s="44"/>
+      <c r="AA5" s="44"/>
+      <c r="AB5" s="44"/>
+      <c r="AC5" s="31"/>
+      <c r="AD5" s="44"/>
+      <c r="AF5" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="AG5" s="39" t="s">
+      <c r="AG5" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="AI5" s="55" t="s">
+      <c r="AI5" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="AJ5" s="39" t="s">
+      <c r="AJ5" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL5" s="39" t="s">
+      <c r="AL5" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="AO5" s="69" t="s">
+      <c r="AO5" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR5" s="70"/>
-    </row>
-    <row r="6" spans="2:48" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="50" t="s">
+      <c r="AR5" s="59"/>
+    </row>
+    <row r="6" spans="2:48" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="41" t="s">
         <v>192</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="42" t="s">
         <v>301</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="F6" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="39" t="s">
+      <c r="F6" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="53"/>
-      <c r="I6" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K6" s="53" t="s">
+      <c r="H6" s="43"/>
+      <c r="I6" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L6" s="54" t="s">
+      <c r="L6" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M6" s="54" t="s">
+      <c r="M6" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N6" s="52"/>
-      <c r="O6" s="56"/>
-      <c r="P6" s="40"/>
-      <c r="Q6" s="54"/>
-      <c r="R6" s="54"/>
-      <c r="S6" s="54"/>
-      <c r="T6" s="54"/>
-      <c r="U6" s="54"/>
-      <c r="V6" s="54"/>
-      <c r="W6" s="54"/>
-      <c r="X6" s="54"/>
-      <c r="Y6" s="54"/>
-      <c r="Z6" s="54"/>
-      <c r="AA6" s="54"/>
-      <c r="AB6" s="54"/>
-      <c r="AC6" s="41"/>
-      <c r="AD6" s="54"/>
-      <c r="AF6" s="39" t="s">
+      <c r="N6" s="42"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="44"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="44"/>
+      <c r="V6" s="44"/>
+      <c r="W6" s="44"/>
+      <c r="X6" s="44"/>
+      <c r="Y6" s="44"/>
+      <c r="Z6" s="44"/>
+      <c r="AA6" s="44"/>
+      <c r="AB6" s="44"/>
+      <c r="AC6" s="31"/>
+      <c r="AD6" s="44"/>
+      <c r="AF6" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="AG6" s="39" t="s">
+      <c r="AG6" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="AI6" s="55" t="s">
+      <c r="AI6" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="AJ6" s="39" t="s">
+      <c r="AJ6" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL6" s="39" t="s">
+      <c r="AL6" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="AO6" s="69" t="s">
+      <c r="AO6" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR6" s="70"/>
-    </row>
-    <row r="7" spans="2:48" s="69" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="74" t="s">
+      <c r="AR6" s="59"/>
+    </row>
+    <row r="7" spans="2:48" s="29" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="41" t="s">
         <v>193</v>
       </c>
-      <c r="D7" s="76" t="s">
+      <c r="D7" s="42" t="s">
         <v>195</v>
       </c>
-      <c r="E7" s="76" t="s">
+      <c r="E7" s="42" t="s">
         <v>196</v>
       </c>
-      <c r="F7" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="69" t="s">
+      <c r="F7" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="77"/>
-      <c r="I7" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" s="77" t="s">
-        <v>54</v>
-      </c>
-      <c r="K7" s="77" t="s">
+      <c r="H7" s="43"/>
+      <c r="I7" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L7" s="79" t="s">
+      <c r="L7" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M7" s="79" t="s">
+      <c r="M7" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N7" s="76"/>
-      <c r="O7" s="80"/>
-      <c r="P7" s="78" t="s">
+      <c r="N7" s="42"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="30" t="s">
         <v>313</v>
       </c>
-      <c r="Q7" s="79"/>
-      <c r="R7" s="79"/>
-      <c r="S7" s="79"/>
-      <c r="T7" s="79"/>
-      <c r="U7" s="79"/>
-      <c r="V7" s="79"/>
-      <c r="W7" s="79"/>
-      <c r="X7" s="79"/>
-      <c r="Y7" s="79"/>
-      <c r="Z7" s="79"/>
-      <c r="AA7" s="79"/>
-      <c r="AB7" s="79"/>
-      <c r="AC7" s="81"/>
-      <c r="AD7" s="79"/>
-      <c r="AF7" s="69" t="s">
+      <c r="Q7" s="44"/>
+      <c r="R7" s="44"/>
+      <c r="S7" s="44"/>
+      <c r="T7" s="44"/>
+      <c r="U7" s="44"/>
+      <c r="V7" s="44"/>
+      <c r="W7" s="44"/>
+      <c r="X7" s="44"/>
+      <c r="Y7" s="44"/>
+      <c r="Z7" s="44"/>
+      <c r="AA7" s="44"/>
+      <c r="AB7" s="44"/>
+      <c r="AC7" s="31"/>
+      <c r="AD7" s="44"/>
+      <c r="AF7" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="AJ7" s="69" t="s">
+      <c r="AJ7" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AO7" s="69" t="s">
+      <c r="AO7" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR7" s="70"/>
-    </row>
-    <row r="8" spans="2:48" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="50" t="s">
+      <c r="AR7" s="59"/>
+    </row>
+    <row r="8" spans="2:48" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="42" t="s">
         <v>199</v>
       </c>
-      <c r="E8" s="52" t="s">
+      <c r="E8" s="42" t="s">
         <v>200</v>
       </c>
-      <c r="F8" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="39" t="s">
+      <c r="F8" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="53"/>
-      <c r="I8" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J8" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K8" s="53" t="s">
+      <c r="H8" s="43"/>
+      <c r="I8" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J8" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L8" s="54" t="s">
+      <c r="L8" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M8" s="54" t="s">
+      <c r="M8" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N8" s="52"/>
-      <c r="O8" s="56"/>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="54"/>
-      <c r="S8" s="54"/>
-      <c r="T8" s="54"/>
-      <c r="U8" s="54"/>
-      <c r="V8" s="54"/>
-      <c r="W8" s="54"/>
-      <c r="X8" s="54"/>
-      <c r="Y8" s="54"/>
-      <c r="Z8" s="54"/>
-      <c r="AA8" s="54"/>
-      <c r="AB8" s="54"/>
-      <c r="AC8" s="41"/>
-      <c r="AD8" s="54"/>
-      <c r="AF8" s="39" t="s">
+      <c r="N8" s="42"/>
+      <c r="O8" s="46"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="44"/>
+      <c r="U8" s="44"/>
+      <c r="V8" s="44"/>
+      <c r="W8" s="44"/>
+      <c r="X8" s="44"/>
+      <c r="Y8" s="44"/>
+      <c r="Z8" s="44"/>
+      <c r="AA8" s="44"/>
+      <c r="AB8" s="44"/>
+      <c r="AC8" s="31"/>
+      <c r="AD8" s="44"/>
+      <c r="AF8" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="AG8" s="39" t="s">
+      <c r="AG8" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="AI8" s="55" t="s">
+      <c r="AI8" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="AJ8" s="39" t="s">
+      <c r="AJ8" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL8" s="39" t="s">
+      <c r="AL8" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="AO8" s="69" t="s">
+      <c r="AO8" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR8" s="70"/>
-    </row>
-    <row r="9" spans="2:48" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="50" t="s">
+      <c r="AR8" s="59"/>
+    </row>
+    <row r="9" spans="2:48" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="41" t="s">
         <v>197</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="D9" s="42" t="s">
         <v>203</v>
       </c>
-      <c r="E9" s="52" t="s">
+      <c r="E9" s="42" t="s">
         <v>204</v>
       </c>
-      <c r="F9" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="69" t="s">
+      <c r="F9" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="53"/>
-      <c r="I9" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J9" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" s="53" t="s">
+      <c r="H9" s="43"/>
+      <c r="I9" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K9" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L9" s="52" t="s">
+      <c r="L9" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="M9" s="54" t="s">
+      <c r="M9" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N9" s="52"/>
-      <c r="O9" s="56"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="54"/>
-      <c r="R9" s="54"/>
-      <c r="S9" s="54"/>
-      <c r="T9" s="54"/>
-      <c r="U9" s="54"/>
-      <c r="V9" s="54"/>
-      <c r="W9" s="54"/>
-      <c r="X9" s="54"/>
-      <c r="Y9" s="54"/>
-      <c r="Z9" s="54"/>
-      <c r="AA9" s="54"/>
-      <c r="AB9" s="54"/>
-      <c r="AC9" s="41"/>
-      <c r="AD9" s="54"/>
-      <c r="AF9" s="39" t="s">
+      <c r="N9" s="42"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="44"/>
+      <c r="R9" s="44"/>
+      <c r="S9" s="44"/>
+      <c r="T9" s="44"/>
+      <c r="U9" s="44"/>
+      <c r="V9" s="44"/>
+      <c r="W9" s="44"/>
+      <c r="X9" s="44"/>
+      <c r="Y9" s="44"/>
+      <c r="Z9" s="44"/>
+      <c r="AA9" s="44"/>
+      <c r="AB9" s="44"/>
+      <c r="AC9" s="31"/>
+      <c r="AD9" s="44"/>
+      <c r="AF9" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="AG9" s="39" t="s">
+      <c r="AG9" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="AI9" s="55" t="s">
+      <c r="AI9" s="45" t="s">
         <v>241</v>
       </c>
-      <c r="AJ9" s="39" t="s">
+      <c r="AJ9" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL9" s="39" t="s">
+      <c r="AL9" s="29" t="s">
         <v>245</v>
       </c>
-      <c r="AO9" s="69" t="s">
+      <c r="AO9" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR9" s="70"/>
-    </row>
-    <row r="10" spans="2:48" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="50" t="s">
+      <c r="AR9" s="59"/>
+    </row>
+    <row r="10" spans="2:48" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="41" t="s">
         <v>198</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="42" t="s">
         <v>207</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="F10" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="39" t="s">
+      <c r="F10" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="53"/>
-      <c r="I10" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="J10" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" s="53" t="s">
+      <c r="H10" s="43"/>
+      <c r="I10" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L10" s="54" t="s">
+      <c r="L10" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M10" s="54" t="s">
+      <c r="M10" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N10" s="52"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="40" t="s">
+      <c r="N10" s="42"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="Q10" s="54"/>
-      <c r="R10" s="54"/>
-      <c r="S10" s="54"/>
-      <c r="T10" s="54"/>
-      <c r="U10" s="54"/>
-      <c r="V10" s="54"/>
-      <c r="W10" s="54"/>
-      <c r="X10" s="54"/>
-      <c r="Y10" s="54"/>
-      <c r="Z10" s="54"/>
-      <c r="AA10" s="54"/>
-      <c r="AB10" s="54"/>
-      <c r="AC10" s="41"/>
-      <c r="AD10" s="54"/>
-      <c r="AF10" s="39" t="s">
+      <c r="Q10" s="44"/>
+      <c r="R10" s="44"/>
+      <c r="S10" s="44"/>
+      <c r="T10" s="44"/>
+      <c r="U10" s="44"/>
+      <c r="V10" s="44"/>
+      <c r="W10" s="44"/>
+      <c r="X10" s="44"/>
+      <c r="Y10" s="44"/>
+      <c r="Z10" s="44"/>
+      <c r="AA10" s="44"/>
+      <c r="AB10" s="44"/>
+      <c r="AC10" s="31"/>
+      <c r="AD10" s="44"/>
+      <c r="AF10" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="AG10" s="39" t="s">
+      <c r="AG10" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="AI10" s="55" t="s">
+      <c r="AI10" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="AJ10" s="39" t="s">
+      <c r="AJ10" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL10" s="39" t="s">
+      <c r="AL10" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="AO10" s="69" t="s">
+      <c r="AO10" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR10" s="70"/>
-    </row>
-    <row r="11" spans="2:48" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="50" t="s">
+      <c r="AR10" s="59"/>
+    </row>
+    <row r="11" spans="2:48" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="41" t="s">
         <v>206</v>
       </c>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="42" t="s">
         <v>219</v>
       </c>
-      <c r="F11" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="39" t="s">
+      <c r="F11" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="53"/>
-      <c r="I11" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J11" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K11" s="53" t="s">
+      <c r="H11" s="43"/>
+      <c r="I11" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L11" s="54" t="s">
+      <c r="L11" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M11" s="54" t="s">
+      <c r="M11" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N11" s="52"/>
-      <c r="O11" s="56"/>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="54"/>
-      <c r="R11" s="54"/>
-      <c r="S11" s="54"/>
-      <c r="T11" s="54"/>
-      <c r="U11" s="54"/>
-      <c r="V11" s="54"/>
-      <c r="W11" s="54"/>
-      <c r="X11" s="54"/>
-      <c r="Y11" s="54"/>
-      <c r="Z11" s="54"/>
-      <c r="AA11" s="54"/>
-      <c r="AB11" s="54"/>
-      <c r="AC11" s="41"/>
-      <c r="AD11" s="54"/>
-      <c r="AF11" s="39" t="s">
+      <c r="N11" s="42"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="44"/>
+      <c r="S11" s="44"/>
+      <c r="T11" s="44"/>
+      <c r="U11" s="44"/>
+      <c r="V11" s="44"/>
+      <c r="W11" s="44"/>
+      <c r="X11" s="44"/>
+      <c r="Y11" s="44"/>
+      <c r="Z11" s="44"/>
+      <c r="AA11" s="44"/>
+      <c r="AB11" s="44"/>
+      <c r="AC11" s="31"/>
+      <c r="AD11" s="44"/>
+      <c r="AF11" s="29" t="s">
         <v>238</v>
       </c>
-      <c r="AG11" s="39" t="s">
+      <c r="AG11" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="AI11" s="55" t="s">
+      <c r="AI11" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="AJ11" s="39" t="s">
+      <c r="AJ11" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL11" s="39" t="s">
+      <c r="AL11" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="AO11" s="69" t="s">
+      <c r="AO11" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR11" s="70"/>
-    </row>
-    <row r="12" spans="2:48" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="50" t="s">
+      <c r="AR11" s="59"/>
+    </row>
+    <row r="12" spans="2:48" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="D12" s="52" t="s">
+      <c r="D12" s="42" t="s">
         <v>214</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="42" t="s">
         <v>220</v>
       </c>
-      <c r="F12" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="39" t="s">
+      <c r="F12" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="53"/>
-      <c r="I12" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J12" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K12" s="53" t="s">
+      <c r="H12" s="43"/>
+      <c r="I12" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="43" t="s">
         <v>226</v>
       </c>
-      <c r="L12" s="54" t="s">
+      <c r="L12" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M12" s="54" t="s">
+      <c r="M12" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N12" s="52"/>
-      <c r="O12" s="56"/>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="54"/>
-      <c r="R12" s="54"/>
-      <c r="S12" s="54"/>
-      <c r="T12" s="54"/>
-      <c r="U12" s="54"/>
-      <c r="V12" s="54"/>
-      <c r="W12" s="54"/>
-      <c r="X12" s="54"/>
-      <c r="Y12" s="54"/>
-      <c r="Z12" s="54"/>
-      <c r="AA12" s="54"/>
-      <c r="AB12" s="54"/>
-      <c r="AC12" s="41"/>
-      <c r="AD12" s="54"/>
-      <c r="AF12" s="39" t="s">
+      <c r="N12" s="42"/>
+      <c r="O12" s="46"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="44"/>
+      <c r="R12" s="44"/>
+      <c r="S12" s="44"/>
+      <c r="T12" s="44"/>
+      <c r="U12" s="44"/>
+      <c r="V12" s="44"/>
+      <c r="W12" s="44"/>
+      <c r="X12" s="44"/>
+      <c r="Y12" s="44"/>
+      <c r="Z12" s="44"/>
+      <c r="AA12" s="44"/>
+      <c r="AB12" s="44"/>
+      <c r="AC12" s="31"/>
+      <c r="AD12" s="44"/>
+      <c r="AF12" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="AG12" s="39" t="s">
+      <c r="AG12" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="AI12" s="55" t="s">
+      <c r="AI12" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="AJ12" s="39" t="s">
+      <c r="AJ12" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL12" s="39" t="s">
+      <c r="AL12" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="AO12" s="69" t="s">
+      <c r="AO12" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR12" s="70"/>
-    </row>
-    <row r="13" spans="2:48" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="50" t="s">
+      <c r="AR12" s="59"/>
+    </row>
+    <row r="13" spans="2:48" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="41" t="s">
         <v>211</v>
       </c>
-      <c r="D13" s="52" t="s">
+      <c r="D13" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="E13" s="52" t="s">
+      <c r="E13" s="42" t="s">
         <v>221</v>
       </c>
-      <c r="F13" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="39" t="s">
+      <c r="F13" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="53"/>
-      <c r="I13" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J13" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K13" s="53" t="s">
+      <c r="H13" s="43"/>
+      <c r="I13" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J13" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L13" s="52" t="s">
+      <c r="L13" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="M13" s="54" t="s">
+      <c r="M13" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N13" s="52"/>
-      <c r="O13" s="56"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="54"/>
-      <c r="R13" s="54"/>
-      <c r="S13" s="54"/>
-      <c r="T13" s="54"/>
-      <c r="U13" s="54"/>
-      <c r="V13" s="54"/>
-      <c r="W13" s="54"/>
-      <c r="X13" s="54"/>
-      <c r="Y13" s="54"/>
-      <c r="Z13" s="54"/>
-      <c r="AA13" s="54"/>
-      <c r="AB13" s="54"/>
-      <c r="AC13" s="41"/>
-      <c r="AD13" s="54"/>
-      <c r="AF13" s="39" t="s">
+      <c r="N13" s="42"/>
+      <c r="O13" s="46"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="44"/>
+      <c r="S13" s="44"/>
+      <c r="T13" s="44"/>
+      <c r="U13" s="44"/>
+      <c r="V13" s="44"/>
+      <c r="W13" s="44"/>
+      <c r="X13" s="44"/>
+      <c r="Y13" s="44"/>
+      <c r="Z13" s="44"/>
+      <c r="AA13" s="44"/>
+      <c r="AB13" s="44"/>
+      <c r="AC13" s="31"/>
+      <c r="AD13" s="44"/>
+      <c r="AF13" s="29" t="s">
         <v>239</v>
       </c>
-      <c r="AG13" s="39" t="s">
+      <c r="AG13" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="AI13" s="55" t="s">
+      <c r="AI13" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="AJ13" s="39" t="s">
+      <c r="AJ13" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL13" s="39" t="s">
+      <c r="AL13" s="29" t="s">
         <v>246</v>
       </c>
-      <c r="AO13" s="69" t="s">
+      <c r="AO13" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR13" s="70"/>
-    </row>
-    <row r="14" spans="2:48" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="50" t="s">
+      <c r="AR13" s="59"/>
+    </row>
+    <row r="14" spans="2:48" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="C14" s="41" t="s">
         <v>212</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="42" t="s">
         <v>166</v>
       </c>
-      <c r="F14" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="39" t="s">
+      <c r="F14" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="53"/>
-      <c r="I14" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J14" s="53" t="s">
+      <c r="H14" s="43"/>
+      <c r="I14" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="K14" s="53" t="s">
+      <c r="K14" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L14" s="54" t="s">
+      <c r="L14" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M14" s="54" t="s">
+      <c r="M14" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N14" s="52"/>
-      <c r="O14" s="56"/>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="54"/>
-      <c r="S14" s="54"/>
-      <c r="T14" s="54"/>
-      <c r="U14" s="54"/>
-      <c r="V14" s="54"/>
-      <c r="W14" s="54"/>
-      <c r="X14" s="54"/>
-      <c r="Y14" s="54"/>
-      <c r="Z14" s="54"/>
-      <c r="AA14" s="54"/>
-      <c r="AB14" s="54"/>
-      <c r="AC14" s="41"/>
-      <c r="AD14" s="54"/>
-      <c r="AF14" s="39" t="s">
+      <c r="N14" s="42"/>
+      <c r="O14" s="46"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="44"/>
+      <c r="R14" s="44"/>
+      <c r="S14" s="44"/>
+      <c r="T14" s="44"/>
+      <c r="U14" s="44"/>
+      <c r="V14" s="44"/>
+      <c r="W14" s="44"/>
+      <c r="X14" s="44"/>
+      <c r="Y14" s="44"/>
+      <c r="Z14" s="44"/>
+      <c r="AA14" s="44"/>
+      <c r="AB14" s="44"/>
+      <c r="AC14" s="31"/>
+      <c r="AD14" s="44"/>
+      <c r="AF14" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="AG14" s="39" t="s">
+      <c r="AG14" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="AI14" s="55" t="s">
+      <c r="AI14" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="AJ14" s="39" t="s">
+      <c r="AJ14" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL14" s="39" t="s">
+      <c r="AL14" s="29" t="s">
         <v>244</v>
       </c>
-      <c r="AO14" s="69" t="s">
+      <c r="AO14" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AQ14" s="39" t="s">
+      <c r="AQ14" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AR14" s="70"/>
-    </row>
-    <row r="15" spans="2:48" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="50" t="s">
+      <c r="AR14" s="59"/>
+    </row>
+    <row r="15" spans="2:48" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="E15" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="F15" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" s="39" t="s">
+      <c r="F15" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="53"/>
-      <c r="I15" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="J15" s="53" t="s">
+      <c r="H15" s="43"/>
+      <c r="I15" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="K15" s="53" t="s">
+      <c r="K15" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L15" s="54" t="s">
+      <c r="L15" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M15" s="54" t="s">
+      <c r="M15" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N15" s="52"/>
-      <c r="O15" s="56"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="54"/>
-      <c r="R15" s="54"/>
-      <c r="S15" s="54"/>
-      <c r="T15" s="54"/>
-      <c r="U15" s="54"/>
-      <c r="V15" s="54"/>
-      <c r="W15" s="54"/>
-      <c r="X15" s="54"/>
-      <c r="Y15" s="54"/>
-      <c r="Z15" s="54"/>
-      <c r="AA15" s="54"/>
-      <c r="AB15" s="54"/>
-      <c r="AC15" s="41"/>
-      <c r="AD15" s="54"/>
-      <c r="AF15" s="39" t="s">
+      <c r="N15" s="42"/>
+      <c r="O15" s="46"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="44"/>
+      <c r="R15" s="44"/>
+      <c r="S15" s="44"/>
+      <c r="T15" s="44"/>
+      <c r="U15" s="44"/>
+      <c r="V15" s="44"/>
+      <c r="W15" s="44"/>
+      <c r="X15" s="44"/>
+      <c r="Y15" s="44"/>
+      <c r="Z15" s="44"/>
+      <c r="AA15" s="44"/>
+      <c r="AB15" s="44"/>
+      <c r="AC15" s="31"/>
+      <c r="AD15" s="44"/>
+      <c r="AF15" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="AG15" s="39" t="s">
+      <c r="AG15" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="AI15" s="55" t="s">
+      <c r="AI15" s="45" t="s">
         <v>242</v>
       </c>
-      <c r="AJ15" s="39" t="s">
+      <c r="AJ15" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL15" s="39" t="s">
+      <c r="AL15" s="29" t="s">
         <v>243</v>
       </c>
-      <c r="AO15" s="69" t="s">
+      <c r="AO15" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AQ15" s="39" t="s">
+      <c r="AQ15" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AR15" s="70"/>
-    </row>
-    <row r="16" spans="2:48" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="74" t="s">
+      <c r="AR15" s="59"/>
+    </row>
+    <row r="16" spans="2:48" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C16" s="75" t="s">
+      <c r="C16" s="41" t="s">
         <v>223</v>
       </c>
-      <c r="D16" s="76" t="s">
+      <c r="D16" s="42" t="s">
         <v>225</v>
       </c>
-      <c r="E16" s="76" t="s">
+      <c r="E16" s="42" t="s">
         <v>322</v>
       </c>
-      <c r="F16" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="G16" s="69" t="s">
+      <c r="F16" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="77"/>
-      <c r="I16" s="78" t="s">
+      <c r="H16" s="43"/>
+      <c r="I16" s="30" t="s">
         <v>314</v>
       </c>
-      <c r="J16" s="77" t="s">
+      <c r="J16" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="K16" s="53" t="s">
+      <c r="K16" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L16" s="79" t="s">
+      <c r="L16" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M16" s="79" t="s">
+      <c r="M16" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N16" s="76"/>
-      <c r="O16" s="80"/>
-      <c r="P16" s="78"/>
-      <c r="Q16" s="79"/>
-      <c r="R16" s="79"/>
-      <c r="S16" s="79"/>
-      <c r="T16" s="79"/>
-      <c r="U16" s="79"/>
-      <c r="V16" s="79" t="s">
+      <c r="N16" s="42"/>
+      <c r="O16" s="46"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="44"/>
+      <c r="R16" s="44"/>
+      <c r="S16" s="44"/>
+      <c r="T16" s="44"/>
+      <c r="U16" s="44"/>
+      <c r="V16" s="44" t="s">
         <v>315</v>
       </c>
-      <c r="W16" s="79" t="s">
+      <c r="W16" s="44" t="s">
         <v>316</v>
       </c>
-      <c r="X16" s="79"/>
-      <c r="Y16" s="79"/>
-      <c r="Z16" s="79"/>
-      <c r="AA16" s="79"/>
-      <c r="AB16" s="79"/>
-      <c r="AC16" s="81"/>
-      <c r="AD16" s="79"/>
-      <c r="AF16" s="69" t="s">
+      <c r="X16" s="44"/>
+      <c r="Y16" s="44"/>
+      <c r="Z16" s="44"/>
+      <c r="AA16" s="44"/>
+      <c r="AB16" s="44"/>
+      <c r="AC16" s="31"/>
+      <c r="AD16" s="44"/>
+      <c r="AF16" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="AG16" s="69" t="s">
+      <c r="AG16" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="AI16" s="82"/>
-      <c r="AJ16" s="69" t="s">
+      <c r="AI16" s="45"/>
+      <c r="AJ16" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AO16" s="69" t="s">
+      <c r="AO16" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AQ16" s="69" t="s">
+      <c r="AQ16" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AR16" s="70"/>
-    </row>
-    <row r="17" spans="2:59" s="62" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="59" t="s">
+      <c r="AR16" s="59"/>
+    </row>
+    <row r="17" spans="2:44" s="52" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="49" t="s">
         <v>189</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="50" t="s">
         <v>224</v>
       </c>
-      <c r="D17" s="61" t="s">
+      <c r="D17" s="51" t="s">
         <v>308</v>
       </c>
-      <c r="E17" s="61" t="s">
+      <c r="E17" s="51" t="s">
         <v>307</v>
       </c>
-      <c r="F17" s="62" t="s">
+      <c r="F17" s="52" t="s">
         <v>228</v>
       </c>
-      <c r="G17" s="62" t="s">
+      <c r="G17" s="52" t="s">
         <v>205</v>
       </c>
-      <c r="H17" s="63"/>
-      <c r="I17" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="J17" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="K17" s="61" t="s">
+      <c r="H17" s="53"/>
+      <c r="I17" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="J17" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="K17" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="L17" s="61" t="s">
+      <c r="L17" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="M17" s="64" t="s">
+      <c r="M17" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="N17" s="61"/>
-      <c r="O17" s="65"/>
-      <c r="P17" s="66"/>
-      <c r="Q17" s="64"/>
-      <c r="R17" s="64"/>
-      <c r="S17" s="64"/>
-      <c r="T17" s="64"/>
-      <c r="U17" s="64"/>
-      <c r="V17" s="64"/>
-      <c r="W17" s="64"/>
-      <c r="X17" s="64"/>
-      <c r="Y17" s="64"/>
-      <c r="Z17" s="64"/>
-      <c r="AA17" s="64"/>
-      <c r="AB17" s="64"/>
-      <c r="AC17" s="67"/>
-      <c r="AD17" s="64"/>
-      <c r="AF17" s="62" t="s">
+      <c r="N17" s="51"/>
+      <c r="O17" s="55"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="54"/>
+      <c r="S17" s="54"/>
+      <c r="T17" s="54"/>
+      <c r="U17" s="54"/>
+      <c r="V17" s="54"/>
+      <c r="W17" s="54"/>
+      <c r="X17" s="54"/>
+      <c r="Y17" s="54"/>
+      <c r="Z17" s="54"/>
+      <c r="AA17" s="54"/>
+      <c r="AB17" s="54"/>
+      <c r="AC17" s="57"/>
+      <c r="AD17" s="54"/>
+      <c r="AF17" s="52" t="s">
         <v>306</v>
       </c>
-      <c r="AG17" s="62" t="s">
+      <c r="AG17" s="52" t="s">
         <v>247</v>
       </c>
-      <c r="AI17" s="68"/>
-      <c r="AJ17" s="39" t="s">
+      <c r="AI17" s="58"/>
+      <c r="AJ17" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL17" s="62" t="s">
+      <c r="AL17" s="52" t="s">
         <v>246</v>
       </c>
-      <c r="AO17" s="62" t="s">
+      <c r="AO17" s="52" t="s">
         <v>173</v>
       </c>
-      <c r="AR17" s="70"/>
-    </row>
-    <row r="18" spans="2:59" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="50" t="s">
+      <c r="AR17" s="59"/>
+    </row>
+    <row r="18" spans="2:44" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="41" t="s">
         <v>227</v>
       </c>
-      <c r="D18" s="52" t="s">
+      <c r="D18" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="E18" s="52" t="s">
+      <c r="E18" s="42" t="s">
         <v>231</v>
       </c>
-      <c r="F18" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" s="54" t="s">
+      <c r="F18" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="52" t="s">
+      <c r="H18" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="I18" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J18" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K18" s="53" t="s">
+      <c r="I18" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J18" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K18" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L18" s="54" t="s">
+      <c r="L18" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M18" s="54" t="s">
+      <c r="M18" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N18" s="52"/>
-      <c r="O18" s="56"/>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="54"/>
-      <c r="R18" s="54"/>
-      <c r="S18" s="54"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="54"/>
-      <c r="V18" s="54"/>
-      <c r="W18" s="54"/>
-      <c r="X18" s="54"/>
-      <c r="Y18" s="54"/>
-      <c r="Z18" s="54"/>
-      <c r="AA18" s="54"/>
-      <c r="AB18" s="54"/>
-      <c r="AC18" s="41"/>
-      <c r="AD18" s="54"/>
-      <c r="AI18" s="55"/>
-      <c r="AJ18" s="39" t="s">
+      <c r="N18" s="42"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="44"/>
+      <c r="R18" s="44"/>
+      <c r="S18" s="44"/>
+      <c r="T18" s="44"/>
+      <c r="U18" s="44"/>
+      <c r="V18" s="44"/>
+      <c r="W18" s="44"/>
+      <c r="X18" s="44"/>
+      <c r="Y18" s="44"/>
+      <c r="Z18" s="44"/>
+      <c r="AA18" s="44"/>
+      <c r="AB18" s="44"/>
+      <c r="AC18" s="31"/>
+      <c r="AD18" s="44"/>
+      <c r="AI18" s="45"/>
+      <c r="AJ18" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AO18" s="69" t="s">
+      <c r="AO18" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR18" s="70"/>
-    </row>
-    <row r="19" spans="2:59" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="50" t="s">
+      <c r="AR18" s="59"/>
+    </row>
+    <row r="19" spans="2:44" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C19" s="51" t="s">
+      <c r="C19" s="41" t="s">
         <v>233</v>
       </c>
-      <c r="D19" s="52" t="s">
+      <c r="D19" s="42" t="s">
         <v>230</v>
       </c>
-      <c r="E19" s="52" t="s">
+      <c r="E19" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="F19" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G19" s="54" t="s">
+      <c r="F19" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="52" t="s">
+      <c r="H19" s="42" t="s">
         <v>230</v>
       </c>
-      <c r="I19" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J19" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K19" s="53" t="s">
+      <c r="I19" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J19" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K19" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L19" s="54" t="s">
+      <c r="L19" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M19" s="54" t="s">
+      <c r="M19" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N19" s="52"/>
-      <c r="O19" s="56"/>
-      <c r="P19" s="40"/>
-      <c r="Q19" s="54"/>
-      <c r="R19" s="54"/>
-      <c r="S19" s="54"/>
-      <c r="T19" s="54"/>
-      <c r="U19" s="54"/>
-      <c r="V19" s="54"/>
-      <c r="W19" s="54"/>
-      <c r="X19" s="54"/>
-      <c r="Y19" s="54"/>
-      <c r="Z19" s="54"/>
-      <c r="AA19" s="54"/>
-      <c r="AB19" s="54"/>
-      <c r="AC19" s="41"/>
-      <c r="AD19" s="54"/>
-      <c r="AI19" s="55"/>
-      <c r="AJ19" s="39" t="s">
+      <c r="N19" s="42"/>
+      <c r="O19" s="46"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="44"/>
+      <c r="R19" s="44"/>
+      <c r="S19" s="44"/>
+      <c r="T19" s="44"/>
+      <c r="U19" s="44"/>
+      <c r="V19" s="44"/>
+      <c r="W19" s="44"/>
+      <c r="X19" s="44"/>
+      <c r="Y19" s="44"/>
+      <c r="Z19" s="44"/>
+      <c r="AA19" s="44"/>
+      <c r="AB19" s="44"/>
+      <c r="AC19" s="31"/>
+      <c r="AD19" s="44"/>
+      <c r="AI19" s="45"/>
+      <c r="AJ19" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AO19" s="69" t="s">
+      <c r="AO19" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR19" s="70"/>
-    </row>
-    <row r="20" spans="2:59" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="50"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="52"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="53"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53" t="s">
+      <c r="AR19" s="59"/>
+    </row>
+    <row r="20" spans="2:44" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="40"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L20" s="54"/>
-      <c r="M20" s="54"/>
-      <c r="N20" s="52"/>
-      <c r="O20" s="56"/>
-      <c r="P20" s="40"/>
-      <c r="Q20" s="54"/>
-      <c r="R20" s="54"/>
-      <c r="S20" s="54"/>
-      <c r="T20" s="54"/>
-      <c r="U20" s="54"/>
-      <c r="V20" s="54"/>
-      <c r="W20" s="54"/>
-      <c r="X20" s="54"/>
-      <c r="Y20" s="54"/>
-      <c r="Z20" s="54"/>
-      <c r="AA20" s="54"/>
-      <c r="AB20" s="54"/>
-      <c r="AC20" s="41"/>
-      <c r="AD20" s="54"/>
-      <c r="AI20" s="55"/>
-      <c r="AJ20" s="39" t="s">
+      <c r="L20" s="44"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="44"/>
+      <c r="R20" s="44"/>
+      <c r="S20" s="44"/>
+      <c r="T20" s="44"/>
+      <c r="U20" s="44"/>
+      <c r="V20" s="44"/>
+      <c r="W20" s="44"/>
+      <c r="X20" s="44"/>
+      <c r="Y20" s="44"/>
+      <c r="Z20" s="44"/>
+      <c r="AA20" s="44"/>
+      <c r="AB20" s="44"/>
+      <c r="AC20" s="31"/>
+      <c r="AD20" s="44"/>
+      <c r="AI20" s="45"/>
+      <c r="AJ20" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AO20" s="69" t="s">
+      <c r="AO20" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR20" s="70"/>
-    </row>
-    <row r="21" spans="2:59" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="50" t="s">
+      <c r="AR20" s="59"/>
+    </row>
+    <row r="21" spans="2:44" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C21" s="51" t="s">
+      <c r="C21" s="41" t="s">
         <v>248</v>
       </c>
-      <c r="D21" s="52" t="s">
+      <c r="D21" s="42" t="s">
         <v>257</v>
       </c>
-      <c r="E21" s="52" t="s">
+      <c r="E21" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="F21" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" s="54" t="s">
+      <c r="F21" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="52"/>
-      <c r="I21" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J21" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K21" s="53" t="s">
+      <c r="H21" s="42"/>
+      <c r="I21" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J21" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K21" s="43" t="s">
         <v>284</v>
       </c>
-      <c r="L21" s="54" t="s">
+      <c r="L21" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M21" s="54" t="s">
+      <c r="M21" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N21" s="52"/>
-      <c r="O21" s="56"/>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="54"/>
-      <c r="R21" s="54"/>
-      <c r="S21" s="54"/>
-      <c r="T21" s="54"/>
-      <c r="U21" s="54"/>
-      <c r="V21" s="54"/>
-      <c r="W21" s="54"/>
-      <c r="X21" s="54"/>
-      <c r="Y21" s="54"/>
-      <c r="Z21" s="54"/>
-      <c r="AA21" s="54"/>
-      <c r="AB21" s="54"/>
-      <c r="AC21" s="41"/>
-      <c r="AD21" s="54"/>
-      <c r="AF21" s="39" t="s">
+      <c r="N21" s="42"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="44"/>
+      <c r="R21" s="44"/>
+      <c r="S21" s="44"/>
+      <c r="T21" s="44"/>
+      <c r="U21" s="44"/>
+      <c r="V21" s="44"/>
+      <c r="W21" s="44"/>
+      <c r="X21" s="44"/>
+      <c r="Y21" s="44"/>
+      <c r="Z21" s="44"/>
+      <c r="AA21" s="44"/>
+      <c r="AB21" s="44"/>
+      <c r="AC21" s="31"/>
+      <c r="AD21" s="44"/>
+      <c r="AF21" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="AG21" s="39" t="s">
+      <c r="AG21" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="AI21" s="55" t="s">
+      <c r="AI21" s="45" t="s">
         <v>283</v>
       </c>
-      <c r="AJ21" s="39" t="s">
+      <c r="AJ21" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL21" s="39" t="s">
+      <c r="AL21" s="29" t="s">
         <v>295</v>
       </c>
-      <c r="AO21" s="69" t="s">
+      <c r="AO21" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR21" s="70"/>
-    </row>
-    <row r="22" spans="2:59" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="50" t="s">
+      <c r="AR21" s="59"/>
+    </row>
+    <row r="22" spans="2:44" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C22" s="51" t="s">
+      <c r="C22" s="41" t="s">
         <v>249</v>
       </c>
-      <c r="D22" s="52" t="s">
+      <c r="D22" s="42" t="s">
         <v>258</v>
       </c>
-      <c r="E22" s="52" t="s">
+      <c r="E22" s="42" t="s">
         <v>260</v>
       </c>
-      <c r="F22" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="54" t="s">
+      <c r="F22" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="52"/>
-      <c r="I22" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J22" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K22" s="53" t="s">
+      <c r="H22" s="42"/>
+      <c r="I22" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J22" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K22" s="43" t="s">
         <v>284</v>
       </c>
-      <c r="L22" s="54" t="s">
+      <c r="L22" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M22" s="54" t="s">
+      <c r="M22" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N22" s="52"/>
-      <c r="O22" s="56"/>
-      <c r="P22" s="40"/>
-      <c r="Q22" s="54"/>
-      <c r="R22" s="54"/>
-      <c r="S22" s="54"/>
-      <c r="T22" s="54"/>
-      <c r="U22" s="54"/>
-      <c r="V22" s="54"/>
-      <c r="W22" s="54"/>
-      <c r="X22" s="54"/>
-      <c r="Y22" s="54"/>
-      <c r="Z22" s="54"/>
-      <c r="AA22" s="54"/>
-      <c r="AB22" s="54"/>
-      <c r="AC22" s="41"/>
-      <c r="AD22" s="54"/>
-      <c r="AF22" s="69" t="s">
+      <c r="N22" s="42"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="44"/>
+      <c r="R22" s="44"/>
+      <c r="S22" s="44"/>
+      <c r="T22" s="44"/>
+      <c r="U22" s="44"/>
+      <c r="V22" s="44"/>
+      <c r="W22" s="44"/>
+      <c r="X22" s="44"/>
+      <c r="Y22" s="44"/>
+      <c r="Z22" s="44"/>
+      <c r="AA22" s="44"/>
+      <c r="AB22" s="44"/>
+      <c r="AC22" s="31"/>
+      <c r="AD22" s="44"/>
+      <c r="AF22" s="29" t="s">
         <v>309</v>
       </c>
-      <c r="AG22" s="39" t="s">
+      <c r="AG22" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="AI22" s="55" t="s">
+      <c r="AI22" s="45" t="s">
         <v>283</v>
       </c>
-      <c r="AJ22" s="39" t="s">
+      <c r="AJ22" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL22" s="39" t="s">
+      <c r="AL22" s="29" t="s">
         <v>295</v>
       </c>
-      <c r="AO22" s="69" t="s">
+      <c r="AO22" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR22" s="70"/>
-    </row>
-    <row r="23" spans="2:59" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="50" t="s">
+      <c r="AR22" s="59"/>
+    </row>
+    <row r="23" spans="2:44" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="C23" s="41" t="s">
         <v>250</v>
       </c>
-      <c r="D23" s="52" t="s">
+      <c r="D23" s="42" t="s">
         <v>261</v>
       </c>
-      <c r="E23" s="52" t="s">
+      <c r="E23" s="42" t="s">
         <v>275</v>
       </c>
-      <c r="F23" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" s="54"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J23" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K23" s="53" t="s">
+      <c r="F23" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="44"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J23" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K23" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L23" s="54" t="s">
+      <c r="L23" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M23" s="54" t="s">
+      <c r="M23" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N23" s="52"/>
-      <c r="O23" s="56"/>
-      <c r="P23" s="40"/>
-      <c r="Q23" s="54"/>
-      <c r="R23" s="54"/>
-      <c r="S23" s="54"/>
-      <c r="T23" s="54"/>
-      <c r="U23" s="54"/>
-      <c r="V23" s="54"/>
-      <c r="W23" s="54"/>
-      <c r="X23" s="54"/>
-      <c r="Y23" s="54"/>
-      <c r="Z23" s="54"/>
-      <c r="AA23" s="54"/>
-      <c r="AB23" s="54"/>
-      <c r="AC23" s="41"/>
-      <c r="AD23" s="54"/>
-      <c r="AF23" s="69" t="s">
+      <c r="N23" s="42"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="44"/>
+      <c r="R23" s="44"/>
+      <c r="S23" s="44"/>
+      <c r="T23" s="44"/>
+      <c r="U23" s="44"/>
+      <c r="V23" s="44"/>
+      <c r="W23" s="44"/>
+      <c r="X23" s="44"/>
+      <c r="Y23" s="44"/>
+      <c r="Z23" s="44"/>
+      <c r="AA23" s="44"/>
+      <c r="AB23" s="44"/>
+      <c r="AC23" s="31"/>
+      <c r="AD23" s="44"/>
+      <c r="AF23" s="29" t="s">
         <v>276</v>
       </c>
-      <c r="AG23" s="39" t="s">
+      <c r="AG23" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="AI23" s="55" t="s">
+      <c r="AI23" s="45" t="s">
         <v>278</v>
       </c>
-      <c r="AJ23" s="39" t="s">
+      <c r="AJ23" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL23" s="39" t="s">
+      <c r="AL23" s="29" t="s">
         <v>293</v>
       </c>
-      <c r="AO23" s="69" t="s">
+      <c r="AO23" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR23" s="70"/>
-    </row>
-    <row r="24" spans="2:59" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="50" t="s">
+      <c r="AR23" s="59"/>
+    </row>
+    <row r="24" spans="2:44" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C24" s="51" t="s">
+      <c r="C24" s="41" t="s">
         <v>251</v>
       </c>
-      <c r="D24" s="52" t="s">
+      <c r="D24" s="42" t="s">
         <v>262</v>
       </c>
-      <c r="E24" s="52" t="s">
+      <c r="E24" s="42" t="s">
         <v>274</v>
       </c>
-      <c r="F24" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" s="54" t="s">
+      <c r="F24" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="H24" s="52"/>
-      <c r="I24" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J24" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K24" s="53" t="s">
+      <c r="H24" s="42"/>
+      <c r="I24" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J24" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K24" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L24" s="54" t="s">
+      <c r="L24" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M24" s="54" t="s">
+      <c r="M24" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N24" s="52"/>
-      <c r="O24" s="56"/>
-      <c r="P24" s="40"/>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="54"/>
-      <c r="S24" s="54"/>
-      <c r="T24" s="54"/>
-      <c r="U24" s="54"/>
-      <c r="V24" s="54"/>
-      <c r="W24" s="54"/>
-      <c r="X24" s="54"/>
-      <c r="Y24" s="54"/>
-      <c r="Z24" s="54"/>
-      <c r="AA24" s="54"/>
-      <c r="AB24" s="54"/>
-      <c r="AC24" s="41"/>
-      <c r="AD24" s="54"/>
-      <c r="AF24" s="69" t="s">
+      <c r="N24" s="42"/>
+      <c r="O24" s="46"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="44"/>
+      <c r="R24" s="44"/>
+      <c r="S24" s="44"/>
+      <c r="T24" s="44"/>
+      <c r="U24" s="44"/>
+      <c r="V24" s="44"/>
+      <c r="W24" s="44"/>
+      <c r="X24" s="44"/>
+      <c r="Y24" s="44"/>
+      <c r="Z24" s="44"/>
+      <c r="AA24" s="44"/>
+      <c r="AB24" s="44"/>
+      <c r="AC24" s="31"/>
+      <c r="AD24" s="44"/>
+      <c r="AF24" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="AG24" s="39" t="s">
+      <c r="AG24" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="AI24" s="55" t="s">
+      <c r="AI24" s="45" t="s">
         <v>279</v>
       </c>
-      <c r="AJ24" s="39" t="s">
+      <c r="AJ24" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL24" s="39" t="s">
+      <c r="AL24" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="AO24" s="69" t="s">
+      <c r="AO24" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR24" s="70"/>
-    </row>
-    <row r="25" spans="2:59" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="50" t="s">
+      <c r="AR24" s="59"/>
+    </row>
+    <row r="25" spans="2:44" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C25" s="51" t="s">
+      <c r="C25" s="41" t="s">
         <v>252</v>
       </c>
-      <c r="D25" s="52" t="s">
+      <c r="D25" s="42" t="s">
         <v>263</v>
       </c>
-      <c r="E25" s="52" t="s">
+      <c r="E25" s="42" t="s">
         <v>272</v>
       </c>
-      <c r="F25" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" s="54" t="s">
+      <c r="F25" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="44" t="s">
         <v>205</v>
       </c>
-      <c r="H25" s="52"/>
-      <c r="I25" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J25" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K25" s="53" t="s">
+      <c r="H25" s="42"/>
+      <c r="I25" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J25" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K25" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L25" s="54" t="s">
+      <c r="L25" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M25" s="54" t="s">
+      <c r="M25" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N25" s="52"/>
-      <c r="O25" s="56"/>
-      <c r="P25" s="40"/>
-      <c r="Q25" s="54"/>
-      <c r="R25" s="54"/>
-      <c r="S25" s="54"/>
-      <c r="T25" s="54"/>
-      <c r="U25" s="54"/>
-      <c r="V25" s="54"/>
-      <c r="W25" s="54"/>
-      <c r="X25" s="54"/>
-      <c r="Y25" s="54"/>
-      <c r="Z25" s="54"/>
-      <c r="AA25" s="54"/>
-      <c r="AB25" s="54"/>
-      <c r="AC25" s="41"/>
-      <c r="AD25" s="54"/>
-      <c r="AF25" s="39" t="s">
+      <c r="N25" s="42"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="30"/>
+      <c r="Q25" s="44"/>
+      <c r="R25" s="44"/>
+      <c r="S25" s="44"/>
+      <c r="T25" s="44"/>
+      <c r="U25" s="44"/>
+      <c r="V25" s="44"/>
+      <c r="W25" s="44"/>
+      <c r="X25" s="44"/>
+      <c r="Y25" s="44"/>
+      <c r="Z25" s="44"/>
+      <c r="AA25" s="44"/>
+      <c r="AB25" s="44"/>
+      <c r="AC25" s="31"/>
+      <c r="AD25" s="44"/>
+      <c r="AF25" s="29" t="s">
         <v>285</v>
       </c>
-      <c r="AG25" s="39" t="s">
+      <c r="AG25" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="AI25" s="55" t="s">
+      <c r="AI25" s="45" t="s">
         <v>279</v>
       </c>
-      <c r="AJ25" s="39" t="s">
+      <c r="AJ25" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL25" s="39" t="s">
+      <c r="AL25" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="AO25" s="69" t="s">
+      <c r="AO25" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR25" s="70"/>
-    </row>
-    <row r="26" spans="2:59" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="50" t="s">
+      <c r="AR25" s="59"/>
+    </row>
+    <row r="26" spans="2:44" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C26" s="51" t="s">
+      <c r="C26" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="D26" s="52" t="s">
+      <c r="D26" s="42" t="s">
         <v>264</v>
       </c>
-      <c r="E26" s="52" t="s">
+      <c r="E26" s="42" t="s">
         <v>273</v>
       </c>
-      <c r="F26" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G26" s="54" t="s">
+      <c r="F26" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="H26" s="52"/>
-      <c r="I26" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J26" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K26" s="53" t="s">
+      <c r="H26" s="42"/>
+      <c r="I26" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J26" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L26" s="54" t="s">
+      <c r="L26" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M26" s="54" t="s">
+      <c r="M26" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N26" s="52"/>
-      <c r="O26" s="56"/>
-      <c r="P26" s="40"/>
-      <c r="Q26" s="54"/>
-      <c r="R26" s="54"/>
-      <c r="S26" s="54"/>
-      <c r="T26" s="54"/>
-      <c r="U26" s="54"/>
-      <c r="V26" s="54"/>
-      <c r="W26" s="54"/>
-      <c r="X26" s="54"/>
-      <c r="Y26" s="54"/>
-      <c r="Z26" s="54"/>
-      <c r="AA26" s="54"/>
-      <c r="AB26" s="54"/>
-      <c r="AC26" s="41"/>
-      <c r="AD26" s="54"/>
-      <c r="AF26" s="39" t="s">
+      <c r="N26" s="42"/>
+      <c r="O26" s="46"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="44"/>
+      <c r="T26" s="44"/>
+      <c r="U26" s="44"/>
+      <c r="V26" s="44"/>
+      <c r="W26" s="44"/>
+      <c r="X26" s="44"/>
+      <c r="Y26" s="44"/>
+      <c r="Z26" s="44"/>
+      <c r="AA26" s="44"/>
+      <c r="AB26" s="44"/>
+      <c r="AC26" s="31"/>
+      <c r="AD26" s="44"/>
+      <c r="AF26" s="29" t="s">
         <v>311</v>
       </c>
-      <c r="AG26" s="39" t="s">
+      <c r="AG26" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="AI26" s="55" t="s">
+      <c r="AI26" s="45" t="s">
         <v>279</v>
       </c>
-      <c r="AJ26" s="39" t="s">
+      <c r="AJ26" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL26" s="39" t="s">
+      <c r="AL26" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="AO26" s="69" t="s">
+      <c r="AO26" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR26" s="70"/>
-    </row>
-    <row r="27" spans="2:59" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="74" t="s">
+      <c r="AR26" s="59"/>
+    </row>
+    <row r="27" spans="2:44" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C27" s="75" t="s">
+      <c r="C27" s="41" t="s">
         <v>254</v>
       </c>
-      <c r="D27" s="76" t="s">
+      <c r="D27" s="42" t="s">
         <v>265</v>
       </c>
-      <c r="E27" s="76" t="s">
+      <c r="E27" s="42" t="s">
         <v>319</v>
       </c>
-      <c r="F27" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="G27" s="79" t="s">
+      <c r="F27" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="H27" s="76"/>
-      <c r="I27" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="J27" s="77" t="s">
+      <c r="H27" s="42"/>
+      <c r="I27" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J27" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="K27" s="77" t="s">
+      <c r="K27" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L27" s="79" t="s">
+      <c r="L27" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M27" s="79" t="s">
+      <c r="M27" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N27" s="76"/>
-      <c r="O27" s="80"/>
-      <c r="P27" s="78" t="s">
+      <c r="N27" s="42"/>
+      <c r="O27" s="46"/>
+      <c r="P27" s="30" t="s">
         <v>321</v>
       </c>
-      <c r="Q27" s="79"/>
-      <c r="R27" s="79"/>
-      <c r="S27" s="79"/>
-      <c r="T27" s="79"/>
-      <c r="U27" s="79"/>
-      <c r="V27" s="79"/>
-      <c r="W27" s="79"/>
-      <c r="X27" s="79"/>
-      <c r="Y27" s="79"/>
-      <c r="Z27" s="79"/>
-      <c r="AA27" s="79"/>
-      <c r="AB27" s="79"/>
-      <c r="AC27" s="81"/>
-      <c r="AD27" s="79"/>
-      <c r="AG27" s="69" t="s">
+      <c r="Q27" s="44"/>
+      <c r="R27" s="44"/>
+      <c r="S27" s="44"/>
+      <c r="T27" s="44"/>
+      <c r="U27" s="44"/>
+      <c r="V27" s="44"/>
+      <c r="W27" s="44"/>
+      <c r="X27" s="44"/>
+      <c r="Y27" s="44"/>
+      <c r="Z27" s="44"/>
+      <c r="AA27" s="44"/>
+      <c r="AB27" s="44"/>
+      <c r="AC27" s="31"/>
+      <c r="AD27" s="44"/>
+      <c r="AG27" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="AI27" s="82" t="s">
+      <c r="AI27" s="45" t="s">
         <v>279</v>
       </c>
-      <c r="AJ27" s="69" t="s">
+      <c r="AJ27" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL27" s="69" t="s">
+      <c r="AL27" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="AO27" s="69" t="s">
+      <c r="AO27" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR27" s="70"/>
-    </row>
-    <row r="28" spans="2:59" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="50" t="s">
+      <c r="AR27" s="59"/>
+    </row>
+    <row r="28" spans="2:44" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C28" s="51" t="s">
+      <c r="C28" s="41" t="s">
         <v>255</v>
       </c>
-      <c r="D28" s="52" t="s">
+      <c r="D28" s="42" t="s">
         <v>312</v>
       </c>
-      <c r="E28" s="52" t="s">
+      <c r="E28" s="42" t="s">
         <v>266</v>
       </c>
-      <c r="F28" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="54" t="s">
+      <c r="F28" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="H28" s="52"/>
-      <c r="I28" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J28" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K28" s="53" t="s">
+      <c r="H28" s="42"/>
+      <c r="I28" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J28" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K28" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L28" s="54" t="s">
+      <c r="L28" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M28" s="54" t="s">
+      <c r="M28" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N28" s="52"/>
-      <c r="O28" s="56"/>
-      <c r="P28" s="40"/>
-      <c r="Q28" s="54"/>
-      <c r="R28" s="54"/>
-      <c r="S28" s="54"/>
-      <c r="T28" s="54"/>
-      <c r="U28" s="54"/>
-      <c r="V28" s="54"/>
-      <c r="W28" s="54"/>
-      <c r="X28" s="54"/>
-      <c r="Y28" s="54"/>
-      <c r="Z28" s="54"/>
-      <c r="AA28" s="54"/>
-      <c r="AB28" s="54"/>
-      <c r="AC28" s="41"/>
-      <c r="AD28" s="54"/>
-      <c r="AF28" s="39" t="s">
+      <c r="N28" s="42"/>
+      <c r="O28" s="46"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="44"/>
+      <c r="R28" s="44"/>
+      <c r="S28" s="44"/>
+      <c r="T28" s="44"/>
+      <c r="U28" s="44"/>
+      <c r="V28" s="44"/>
+      <c r="W28" s="44"/>
+      <c r="X28" s="44"/>
+      <c r="Y28" s="44"/>
+      <c r="Z28" s="44"/>
+      <c r="AA28" s="44"/>
+      <c r="AB28" s="44"/>
+      <c r="AC28" s="31"/>
+      <c r="AD28" s="44"/>
+      <c r="AF28" s="29" t="s">
         <v>286</v>
       </c>
-      <c r="AG28" s="39" t="s">
+      <c r="AG28" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="AI28" s="55" t="s">
+      <c r="AI28" s="45" t="s">
         <v>279</v>
       </c>
-      <c r="AJ28" s="39" t="s">
+      <c r="AJ28" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL28" s="39" t="s">
+      <c r="AL28" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="AO28" s="69" t="s">
+      <c r="AO28" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR28" s="70"/>
-      <c r="AS28" s="69"/>
-      <c r="AT28" s="69"/>
-      <c r="AU28" s="69"/>
-      <c r="AV28" s="69"/>
-      <c r="AW28" s="69"/>
-      <c r="AX28" s="69"/>
-      <c r="AY28" s="69"/>
-      <c r="AZ28" s="69"/>
-      <c r="BA28" s="69"/>
-      <c r="BB28" s="69"/>
-      <c r="BC28" s="69"/>
-      <c r="BD28" s="69"/>
-      <c r="BE28" s="69"/>
-      <c r="BF28" s="69"/>
-      <c r="BG28" s="69"/>
-    </row>
-    <row r="29" spans="2:59" s="69" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="74" t="s">
+      <c r="AR28" s="59"/>
+    </row>
+    <row r="29" spans="2:44" s="29" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C29" s="75" t="s">
+      <c r="C29" s="41" t="s">
         <v>256</v>
       </c>
-      <c r="D29" s="76" t="s">
+      <c r="D29" s="42" t="s">
         <v>267</v>
       </c>
-      <c r="E29" s="76"/>
-      <c r="F29" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="G29" s="79" t="s">
+      <c r="E29" s="42"/>
+      <c r="F29" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="76"/>
-      <c r="I29" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="J29" s="77" t="s">
-        <v>54</v>
-      </c>
-      <c r="K29" s="77" t="s">
+      <c r="H29" s="42"/>
+      <c r="I29" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J29" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K29" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L29" s="79" t="s">
+      <c r="L29" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M29" s="79" t="s">
+      <c r="M29" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="N29" s="76"/>
-      <c r="O29" s="80"/>
-      <c r="P29" s="78" t="s">
+      <c r="N29" s="42"/>
+      <c r="O29" s="46"/>
+      <c r="P29" s="30" t="s">
         <v>320</v>
       </c>
-      <c r="Q29" s="79"/>
-      <c r="R29" s="79"/>
-      <c r="S29" s="79"/>
-      <c r="T29" s="79"/>
-      <c r="U29" s="79"/>
-      <c r="V29" s="79"/>
-      <c r="W29" s="79"/>
-      <c r="X29" s="79"/>
-      <c r="Y29" s="79"/>
-      <c r="Z29" s="79"/>
-      <c r="AA29" s="79"/>
-      <c r="AB29" s="79"/>
-      <c r="AC29" s="81"/>
-      <c r="AD29" s="79"/>
-      <c r="AG29" s="69" t="s">
+      <c r="Q29" s="44"/>
+      <c r="R29" s="44"/>
+      <c r="S29" s="44"/>
+      <c r="T29" s="44"/>
+      <c r="U29" s="44"/>
+      <c r="V29" s="44"/>
+      <c r="W29" s="44"/>
+      <c r="X29" s="44"/>
+      <c r="Y29" s="44"/>
+      <c r="Z29" s="44"/>
+      <c r="AA29" s="44"/>
+      <c r="AB29" s="44"/>
+      <c r="AC29" s="31"/>
+      <c r="AD29" s="44"/>
+      <c r="AG29" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="AI29" s="82" t="s">
+      <c r="AI29" s="45" t="s">
         <v>279</v>
       </c>
-      <c r="AJ29" s="69" t="s">
+      <c r="AJ29" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL29" s="69" t="s">
+      <c r="AL29" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="AO29" s="69" t="s">
+      <c r="AO29" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="AR29" s="70"/>
-    </row>
-    <row r="30" spans="2:59" ht="60" x14ac:dyDescent="0.15">
-      <c r="B30" s="50" t="s">
+      <c r="AR29" s="59"/>
+    </row>
+    <row r="30" spans="2:44" ht="60" x14ac:dyDescent="0.15">
+      <c r="B30" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C30" s="51" t="s">
+      <c r="C30" s="41" t="s">
         <v>268</v>
       </c>
-      <c r="D30" s="52" t="s">
+      <c r="D30" s="42" t="s">
         <v>302</v>
       </c>
-      <c r="E30" s="52" t="s">
+      <c r="E30" s="42" t="s">
         <v>289</v>
       </c>
-      <c r="F30" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G30" s="54" t="s">
+      <c r="F30" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G30" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="H30" s="53" t="s">
+      <c r="H30" s="43" t="s">
         <v>290</v>
       </c>
-      <c r="I30" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J30" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K30" s="53" t="s">
+      <c r="I30" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J30" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K30" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L30" s="54" t="s">
+      <c r="L30" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M30" s="54" t="s">
+      <c r="M30" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="AF30" s="39"/>
-      <c r="AG30" s="39" t="s">
+      <c r="AF30" s="29"/>
+      <c r="AG30" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="AH30" s="39"/>
-      <c r="AJ30" s="39" t="s">
+      <c r="AH30" s="29"/>
+      <c r="AJ30" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL30" s="39" t="s">
+      <c r="AL30" s="29" t="s">
         <v>296</v>
       </c>
-      <c r="AO30" s="69" t="s">
+      <c r="AO30" s="29" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="31" spans="2:59" ht="60" x14ac:dyDescent="0.15">
-      <c r="B31" s="50" t="s">
+    <row r="31" spans="2:44" ht="60" x14ac:dyDescent="0.15">
+      <c r="B31" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C31" s="51" t="s">
+      <c r="C31" s="41" t="s">
         <v>269</v>
       </c>
-      <c r="D31" s="52" t="s">
+      <c r="D31" s="42" t="s">
         <v>303</v>
       </c>
-      <c r="E31" s="52" t="s">
+      <c r="E31" s="42" t="s">
         <v>288</v>
       </c>
-      <c r="F31" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G31" s="39"/>
-      <c r="I31" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J31" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K31" s="53" t="s">
+      <c r="F31" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" s="29"/>
+      <c r="I31" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J31" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K31" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L31" s="54" t="s">
+      <c r="L31" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M31" s="54" t="s">
+      <c r="M31" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="N31" s="54" t="s">
+      <c r="N31" s="44" t="s">
         <v>287</v>
       </c>
-      <c r="AF31" s="69" t="s">
+      <c r="AF31" s="29" t="s">
         <v>292</v>
       </c>
-      <c r="AG31" s="39" t="s">
+      <c r="AG31" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="AH31" s="39"/>
-      <c r="AI31" s="55" t="s">
+      <c r="AH31" s="29"/>
+      <c r="AI31" s="45" t="s">
         <v>279</v>
       </c>
-      <c r="AJ31" s="39" t="s">
+      <c r="AJ31" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL31" s="39" t="s">
+      <c r="AL31" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="AO31" s="69" t="s">
+      <c r="AO31" s="29" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="32" spans="2:59" ht="45" x14ac:dyDescent="0.15">
-      <c r="B32" s="50" t="s">
+    <row r="32" spans="2:44" ht="45" x14ac:dyDescent="0.15">
+      <c r="B32" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C32" s="51" t="s">
+      <c r="C32" s="41" t="s">
         <v>270</v>
       </c>
-      <c r="D32" s="52" t="s">
+      <c r="D32" s="42" t="s">
         <v>304</v>
       </c>
-      <c r="E32" s="52"/>
-      <c r="F32" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G32" s="54" t="s">
+      <c r="E32" s="42"/>
+      <c r="F32" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G32" s="44" t="s">
         <v>281</v>
       </c>
-      <c r="H32" s="52"/>
-      <c r="I32" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J32" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K32" s="53" t="s">
+      <c r="H32" s="42"/>
+      <c r="I32" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J32" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K32" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L32" s="54" t="s">
+      <c r="L32" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M32" s="54" t="s">
+      <c r="M32" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="AF32" s="39" t="s">
+      <c r="AF32" s="29" t="s">
         <v>277</v>
       </c>
-      <c r="AG32" s="39" t="s">
+      <c r="AG32" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="AI32" s="55" t="s">
+      <c r="AI32" s="45" t="s">
         <v>278</v>
       </c>
-      <c r="AJ32" s="39" t="s">
+      <c r="AJ32" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AL32" s="39" t="s">
+      <c r="AL32" s="29" t="s">
         <v>293</v>
       </c>
-      <c r="AO32" s="69" t="s">
+      <c r="AO32" s="29" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="33" spans="2:41" ht="59" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="C33" s="51" t="s">
+      <c r="C33" s="41" t="s">
         <v>271</v>
       </c>
-      <c r="D33" s="52" t="s">
+      <c r="D33" s="42" t="s">
         <v>305</v>
       </c>
-      <c r="F33" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="G33" s="54" t="s">
+      <c r="F33" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="I33" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="J33" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="K33" s="53" t="s">
+      <c r="I33" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="J33" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="K33" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="L33" s="54" t="s">
+      <c r="L33" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="M33" s="54" t="s">
+      <c r="M33" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="AF33" s="39" t="s">
+      <c r="AF33" s="29" t="s">
         <v>282</v>
       </c>
-      <c r="AG33" s="39" t="s">
+      <c r="AG33" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="AI33" s="39" t="s">
+      <c r="AI33" s="29" t="s">
         <v>280</v>
       </c>
-      <c r="AJ33" s="39" t="s">
+      <c r="AJ33" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="AO33" s="69" t="s">
+      <c r="AO33" s="29" t="s">
         <v>173</v>
       </c>
     </row>

</xml_diff>